<commit_message>
commenting changes to setup file
</commit_message>
<xml_diff>
--- a/Data/KSR_climate_calc.xlsx
+++ b/Data/KSR_climate_calc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel_anstett/Dropbox/a Papers/North_garden/KSR_North/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel_anstett/Dropbox/a_Papers/North_garden/KSR_North/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB806A07-4C93-A34F-BC52-6586DA1A4849}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1006EFD-8089-CD44-9B63-ED5CFC235668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16540" xr2:uid="{68C5B7C2-FE45-6F4F-AD81-46652D967442}"/>
   </bookViews>
@@ -23,7 +23,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="54">
   <si>
     <t>year_2013</t>
   </si>
@@ -147,75 +151,6 @@
     <t xml:space="preserve">Tave(01) </t>
   </si>
   <si>
-    <t xml:space="preserve">RH </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CMD </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eref </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAR </t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXT </t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMT </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FFP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">eFFP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">bFFP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NFFD </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DD&gt;18 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DD&lt;18 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DD&gt;5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DD&lt;0 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHM </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AHM </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MSP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TD </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCMT </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MWMT </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAT </t>
-  </si>
-  <si>
     <t>Period</t>
   </si>
   <si>
@@ -229,9 +164,6 @@
   </si>
   <si>
     <t>KSR</t>
-  </si>
-  <si>
-    <t>Means (for reference)</t>
   </si>
   <si>
     <t>KSR specific climate for MAT, CMD &amp; RH</t>
@@ -311,10 +243,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -631,83 +562,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8809CD46-23ED-2D49-9D09-8FBF4518497E}">
-  <dimension ref="A1:AA31"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="A28" sqref="A28:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>77</v>
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <f>AVERAGE(L14:N14,O12:Q12,F13:K13)</f>
         <v>7.8500000000000014</v>
       </c>
       <c r="B6">
         <f>J31</f>
-        <v>456</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <f>SUM(L20:N20,O18:Q18,F19:K19)</f>
         <v>121</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <f>AVERAGE(L26:N26,O24:Q24,F25:K25)</f>
         <v>69.041666666666671</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="R7" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="F11" t="s">
         <v>37</v>
@@ -847,10 +778,9 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="L14">
         <f>AVERAGE(L12:L13)</f>
         <v>21.700000000000003</v>
@@ -869,21 +799,21 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="D17" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="E17" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="F17" t="s">
         <v>25</v>
@@ -922,7 +852,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>44.026361000000001</v>
       </c>
@@ -972,7 +902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B19">
         <v>44.026361000000001</v>
       </c>
@@ -1022,9 +952,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>76</v>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="L20">
         <f>AVERAGE(L18:L19)</f>
@@ -1039,23 +969,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="D23" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="E23" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="F23" t="s">
         <v>13</v>
@@ -1094,7 +1024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B24">
         <v>44.026361000000001</v>
       </c>
@@ -1144,7 +1074,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B25">
         <v>44.026361000000001</v>
       </c>
@@ -1194,9 +1124,9 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>76</v>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="L26">
         <f>AVERAGE(L24:L25)</f>
@@ -1211,259 +1141,8 @@
         <v>66.5</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>64</v>
-      </c>
-      <c r="B29" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" t="s">
-        <v>62</v>
-      </c>
-      <c r="D29" t="s">
-        <v>61</v>
-      </c>
-      <c r="E29" t="s">
-        <v>60</v>
-      </c>
-      <c r="F29" t="s">
-        <v>59</v>
-      </c>
-      <c r="G29" t="s">
-        <v>58</v>
-      </c>
-      <c r="H29" t="s">
-        <v>57</v>
-      </c>
-      <c r="I29" t="s">
-        <v>56</v>
-      </c>
-      <c r="J29" t="s">
-        <v>55</v>
-      </c>
-      <c r="K29" t="s">
-        <v>54</v>
-      </c>
-      <c r="L29" t="s">
-        <v>53</v>
-      </c>
-      <c r="M29" t="s">
-        <v>52</v>
-      </c>
-      <c r="N29" t="s">
-        <v>51</v>
-      </c>
-      <c r="O29" t="s">
-        <v>50</v>
-      </c>
-      <c r="P29" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>48</v>
-      </c>
-      <c r="R29" t="s">
-        <v>47</v>
-      </c>
-      <c r="S29" t="s">
-        <v>46</v>
-      </c>
-      <c r="T29" t="s">
-        <v>45</v>
-      </c>
-      <c r="U29" t="s">
-        <v>44</v>
-      </c>
-      <c r="V29" t="s">
-        <v>43</v>
-      </c>
-      <c r="W29" t="s">
-        <v>42</v>
-      </c>
-      <c r="X29" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y29" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z29" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA29" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>44.026361000000001</v>
-      </c>
-      <c r="B30">
-        <v>-79.545063999999996</v>
-      </c>
-      <c r="C30">
-        <v>290</v>
-      </c>
-      <c r="D30" t="s">
-        <v>1</v>
-      </c>
-      <c r="E30">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="F30">
-        <v>22.3</v>
-      </c>
-      <c r="G30">
-        <v>-3.4</v>
-      </c>
-      <c r="H30">
-        <v>25.7</v>
-      </c>
-      <c r="I30">
-        <v>781</v>
-      </c>
-      <c r="J30">
-        <v>422</v>
-      </c>
-      <c r="K30">
-        <v>24.5</v>
-      </c>
-      <c r="L30">
-        <v>53</v>
-      </c>
-      <c r="M30">
-        <v>352</v>
-      </c>
-      <c r="N30">
-        <v>2421</v>
-      </c>
-      <c r="O30">
-        <v>3524</v>
-      </c>
-      <c r="P30">
-        <v>333</v>
-      </c>
-      <c r="Q30">
-        <v>188</v>
-      </c>
-      <c r="R30">
-        <v>126</v>
-      </c>
-      <c r="S30">
-        <v>282</v>
-      </c>
-      <c r="T30">
-        <v>156</v>
-      </c>
-      <c r="U30">
-        <v>53</v>
-      </c>
-      <c r="V30">
-        <v>-31.5</v>
-      </c>
-      <c r="W30">
-        <v>44.9</v>
-      </c>
-      <c r="X30">
-        <v>-9999</v>
-      </c>
-      <c r="Y30">
-        <v>779</v>
-      </c>
-      <c r="Z30">
-        <v>269</v>
-      </c>
-      <c r="AA30">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>44.026361000000001</v>
-      </c>
-      <c r="B31">
-        <v>-79.545063999999996</v>
-      </c>
-      <c r="C31">
-        <v>290</v>
-      </c>
-      <c r="D31" t="s">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>7.2</v>
-      </c>
-      <c r="F31">
-        <v>21.1</v>
-      </c>
-      <c r="G31">
-        <v>-5.7</v>
-      </c>
-      <c r="H31">
-        <v>26.8</v>
-      </c>
-      <c r="I31">
-        <v>964</v>
-      </c>
-      <c r="J31">
-        <v>456</v>
-      </c>
-      <c r="K31">
-        <v>17.899999999999999</v>
-      </c>
-      <c r="L31">
-        <v>46.3</v>
-      </c>
-      <c r="M31">
-        <v>667</v>
-      </c>
-      <c r="N31">
-        <v>2174</v>
-      </c>
-      <c r="O31">
-        <v>4138</v>
-      </c>
-      <c r="P31">
-        <v>247</v>
-      </c>
-      <c r="Q31">
-        <v>186</v>
-      </c>
-      <c r="R31">
-        <v>129</v>
-      </c>
-      <c r="S31">
-        <v>281</v>
-      </c>
-      <c r="T31">
-        <v>153</v>
-      </c>
-      <c r="U31">
-        <v>139</v>
-      </c>
-      <c r="V31">
-        <v>-31.5</v>
-      </c>
-      <c r="W31">
-        <v>44.9</v>
-      </c>
-      <c r="X31">
-        <v>-9999</v>
-      </c>
-      <c r="Y31">
-        <v>681</v>
-      </c>
-      <c r="Z31">
-        <v>101</v>
-      </c>
-      <c r="AA31">
-        <v>68</v>
-      </c>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>